<commit_message>
replace _list.txt with class object
</commit_message>
<xml_diff>
--- a/examples/examples.xlsx
+++ b/examples/examples.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\xampp\htdocs\python\batch_file_handler\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{01E5B776-056B-4753-B94F-2A0D4884E9DF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B1A3437-7D1B-487E-ADEB-5AB1BC958186}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{620FA795-5A76-4A72-B92A-BABDD140C35A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{620FA795-5A76-4A72-B92A-BABDD140C35A}"/>
   </bookViews>
   <sheets>
     <sheet name="Handbrake" sheetId="1" r:id="rId1"/>
     <sheet name="MYOH App" sheetId="2" r:id="rId2"/>
     <sheet name="YouTube-dl 000" sheetId="3" r:id="rId3"/>
+    <sheet name="Name From Date" sheetId="4" r:id="rId4"/>
+    <sheet name="Voice Recorder" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_des">Handbrake!$K$2:$K$8</definedName>
@@ -25,6 +27,13 @@
     <definedName name="_num">Handbrake!$I$2:$I$8</definedName>
     <definedName name="_type">IFERROR(INDEX(_types,MATCH(Handbrake!$E1,_num,0)),"")</definedName>
     <definedName name="_types">Handbrake!$J$2:$J$8</definedName>
+    <definedName name="day">MID(first_word,SEARCH("/",first_word)+1,SEARCH("/",first_word,SEARCH("/",first_word)+1)-SEARCH("/",first_word)-1)</definedName>
+    <definedName name="first_word">LEFT('Name From Date'!$A1,FIND(" ",'Name From Date'!$A1)-1)</definedName>
+    <definedName name="last_word">RIGHT('Name From Date'!$A1,LEN('Name From Date'!$A1)-FIND("*",SUBSTITUTE('Name From Date'!$A1," ","*",LEN('Name From Date'!$A1)-LEN(SUBSTITUTE('Name From Date'!$A1," ","")))))</definedName>
+    <definedName name="month">LEFT(first_word,SEARCH("/",first_word,1)-1)</definedName>
+    <definedName name="month_name">TEXT(DATEVALUE(first_word),"mmm")</definedName>
+    <definedName name="time">TRIM(MID(SUBSTITUTE('Name From Date'!$A1," ",REPT(" ",LEN('Name From Date'!$A1))), (2)*LEN('Name From Date'!$A1)+1, (2)*LEN('Name From Date'!$A1)))</definedName>
+    <definedName name="year">RIGHT(first_word,SEARCH("/",first_word,SEARCH("/",first_word)+1)-2)</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="706">
   <si>
     <t>Old Name</t>
   </si>
@@ -2329,6 +2338,600 @@
   </si>
   <si>
     <t>138 - 'Infertility' Baptist Preaching (independent, fundamental, KJV Bible sermon).mp4</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Long Date</t>
+  </si>
+  <si>
+    <t>12/16/2018  01:34 PM       238,235,648 My Recording_1.wav</t>
+  </si>
+  <si>
+    <t>12/16/2018  10:00 PM       466,536,448 My Recording_3.wav</t>
+  </si>
+  <si>
+    <t>My Recording_3.wav</t>
+  </si>
+  <si>
+    <t>12/17/2018  01:54 PM     2,404,695,552 My Recording_4.wav</t>
+  </si>
+  <si>
+    <t>My Recording_4.wav</t>
+  </si>
+  <si>
+    <t>12/17/2018  04:31 PM     1,484,370,944 My Recording_5.wav</t>
+  </si>
+  <si>
+    <t>My Recording_5.wav</t>
+  </si>
+  <si>
+    <t>12/17/2018  11:32 PM     4,143,924,736 My Recording_6.wav</t>
+  </si>
+  <si>
+    <t>My Recording_6.wav</t>
+  </si>
+  <si>
+    <t>12/18/2018  03:47 PM     2,469,003,264 My Recording_9.wav</t>
+  </si>
+  <si>
+    <t>My Recording_9.wav</t>
+  </si>
+  <si>
+    <t>12/18/2018  06:25 PM     1,504,340,992 My Recording_10.wav</t>
+  </si>
+  <si>
+    <t>My Recording_10.wav</t>
+  </si>
+  <si>
+    <t>12/18/2018  07:20 PM       564,411,904 My Recording_11.wav</t>
+  </si>
+  <si>
+    <t>My Recording_11.wav</t>
+  </si>
+  <si>
+    <t>12/18/2018  11:21 AM     2,597,127,680 My Recording_7.wav</t>
+  </si>
+  <si>
+    <t>My Recording_7.wav</t>
+  </si>
+  <si>
+    <t>12/18/2018  11:54 AM       345,619,456 My Recording_8.wav</t>
+  </si>
+  <si>
+    <t>My Recording_8.wav</t>
+  </si>
+  <si>
+    <t>12/19/2018  01:30 PM       633,855,488 My Recording_15.wav</t>
+  </si>
+  <si>
+    <t>My Recording_15.wav</t>
+  </si>
+  <si>
+    <t>12/19/2018  05:18 PM       951,878,144 My Recording_16.wav</t>
+  </si>
+  <si>
+    <t>My Recording_16.wav</t>
+  </si>
+  <si>
+    <t>12/19/2018  09:50 PM     1,705,134,592 My Recording_17.wav</t>
+  </si>
+  <si>
+    <t>My Recording_17.wav</t>
+  </si>
+  <si>
+    <t>12/19/2018  10:12 AM     1,000,151,040 My Recording_13.wav</t>
+  </si>
+  <si>
+    <t>My Recording_13.wav</t>
+  </si>
+  <si>
+    <t>12/19/2018  12:30 PM         6,633,984 My Recording_14.wav</t>
+  </si>
+  <si>
+    <t>My Recording_14.wav</t>
+  </si>
+  <si>
+    <t>12/19/2018  12:51 AM     3,500,134,400 My Recording_12.wav</t>
+  </si>
+  <si>
+    <t>My Recording_12.wav</t>
+  </si>
+  <si>
+    <t>Voice 021.m4a</t>
+  </si>
+  <si>
+    <t>2017 Nov</t>
+  </si>
+  <si>
+    <t>.m4a</t>
+  </si>
+  <si>
+    <t>Voice 022.m4a</t>
+  </si>
+  <si>
+    <t>Voice 023.m4a</t>
+  </si>
+  <si>
+    <t>Voice 024.m4a</t>
+  </si>
+  <si>
+    <t>Voice 025.m4a</t>
+  </si>
+  <si>
+    <t>Voice 026.m4a</t>
+  </si>
+  <si>
+    <t>Voice 027.m4a</t>
+  </si>
+  <si>
+    <t>Voice 028.m4a</t>
+  </si>
+  <si>
+    <t>2017 Dec</t>
+  </si>
+  <si>
+    <t>Voice 029.m4a</t>
+  </si>
+  <si>
+    <t>Voice 030.m4a</t>
+  </si>
+  <si>
+    <t>Voice 031.m4a</t>
+  </si>
+  <si>
+    <t>Voice 032.m4a</t>
+  </si>
+  <si>
+    <t>Voice 033.m4a</t>
+  </si>
+  <si>
+    <t>Voice 034.m4a</t>
+  </si>
+  <si>
+    <t>Voice 035.m4a</t>
+  </si>
+  <si>
+    <t>Voice 036.m4a</t>
+  </si>
+  <si>
+    <t>Voice 037.m4a</t>
+  </si>
+  <si>
+    <t>Voice 038.m4a</t>
+  </si>
+  <si>
+    <t>Voice 039.m4a</t>
+  </si>
+  <si>
+    <t>Voice 040.m4a</t>
+  </si>
+  <si>
+    <t>Voice 041.m4a</t>
+  </si>
+  <si>
+    <t>Voice 042.m4a</t>
+  </si>
+  <si>
+    <t>Voice 043.m4a</t>
+  </si>
+  <si>
+    <t>Voice 044.m4a</t>
+  </si>
+  <si>
+    <t>Voice 045.m4a</t>
+  </si>
+  <si>
+    <t>Voice 046.m4a</t>
+  </si>
+  <si>
+    <t>Voice 047.m4a</t>
+  </si>
+  <si>
+    <t>Voice 048.m4a</t>
+  </si>
+  <si>
+    <t>Voice 049.m4a</t>
+  </si>
+  <si>
+    <t>2018 Jan</t>
+  </si>
+  <si>
+    <t>Voice 050.m4a</t>
+  </si>
+  <si>
+    <t>Voice 051.m4a</t>
+  </si>
+  <si>
+    <t>Voice 052.m4a</t>
+  </si>
+  <si>
+    <t>Voice 053.m4a</t>
+  </si>
+  <si>
+    <t>Voice 054.m4a</t>
+  </si>
+  <si>
+    <t>Voice 055.m4a</t>
+  </si>
+  <si>
+    <t>Voice 056.m4a</t>
+  </si>
+  <si>
+    <t>Voice 057.m4a</t>
+  </si>
+  <si>
+    <t>2018 Feb</t>
+  </si>
+  <si>
+    <t>Voice 058.m4a</t>
+  </si>
+  <si>
+    <t>Voice 059.m4a</t>
+  </si>
+  <si>
+    <t>Voice 060.m4a</t>
+  </si>
+  <si>
+    <t>Voice 062.m4a</t>
+  </si>
+  <si>
+    <t>Voice 063.m4a</t>
+  </si>
+  <si>
+    <t>Voice 064.m4a</t>
+  </si>
+  <si>
+    <t>Voice 065.m4a</t>
+  </si>
+  <si>
+    <t>Voice 066.m4a</t>
+  </si>
+  <si>
+    <t>Voice 067.m4a</t>
+  </si>
+  <si>
+    <t>Voice 068.m4a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018 Mar </t>
+  </si>
+  <si>
+    <t>Voice 069.m4a</t>
+  </si>
+  <si>
+    <t>Voice 070.m4a</t>
+  </si>
+  <si>
+    <t>Voice 071.m4a</t>
+  </si>
+  <si>
+    <t>Voice 072.m4a</t>
+  </si>
+  <si>
+    <t>Voice 073.m4a</t>
+  </si>
+  <si>
+    <t>Voice 074.m4a</t>
+  </si>
+  <si>
+    <t>Voice 075.m4a</t>
+  </si>
+  <si>
+    <t>Voice 076.m4a</t>
+  </si>
+  <si>
+    <t>Voice 077.m4a</t>
+  </si>
+  <si>
+    <t>Voice 078.m4a</t>
+  </si>
+  <si>
+    <t>Voice 079.m4a</t>
+  </si>
+  <si>
+    <t>2018 Apr</t>
+  </si>
+  <si>
+    <t>Voice 080.m4a</t>
+  </si>
+  <si>
+    <t>2018 May</t>
+  </si>
+  <si>
+    <t>Voice 081.m4a</t>
+  </si>
+  <si>
+    <t>Voice 082.m4a</t>
+  </si>
+  <si>
+    <t>Voice 083.m4a</t>
+  </si>
+  <si>
+    <t>Voice 084.m4a</t>
+  </si>
+  <si>
+    <t>Voice 085.m4a</t>
+  </si>
+  <si>
+    <t>Voice 086.m4a</t>
+  </si>
+  <si>
+    <t>Voice 087.m4a</t>
+  </si>
+  <si>
+    <t>Voice 088.m4a</t>
+  </si>
+  <si>
+    <t>Voice 089.m4a</t>
+  </si>
+  <si>
+    <t>Voice 090.m4a</t>
+  </si>
+  <si>
+    <t>Voice 091.m4a</t>
+  </si>
+  <si>
+    <t>Voice 092.m4a</t>
+  </si>
+  <si>
+    <t>Voice 093.m4a</t>
+  </si>
+  <si>
+    <t>Voice 094.m4a</t>
+  </si>
+  <si>
+    <t>Voice 095.m4a</t>
+  </si>
+  <si>
+    <t>Voice 096.m4a</t>
+  </si>
+  <si>
+    <t>2018 Jun</t>
+  </si>
+  <si>
+    <t>Voice 097.m4a</t>
+  </si>
+  <si>
+    <t>Voice 098.m4a</t>
+  </si>
+  <si>
+    <t>Voice 099.m4a</t>
+  </si>
+  <si>
+    <t>Voice 100.m4a</t>
+  </si>
+  <si>
+    <t>Voice 101.m4a</t>
+  </si>
+  <si>
+    <t>Voice 102.m4a</t>
+  </si>
+  <si>
+    <t>Voice 103.m4a</t>
+  </si>
+  <si>
+    <t>Voice 104.m4a</t>
+  </si>
+  <si>
+    <t>Voice 105.m4a</t>
+  </si>
+  <si>
+    <t>Voice 106.m4a</t>
+  </si>
+  <si>
+    <t>Voice 107.m4a</t>
+  </si>
+  <si>
+    <t>Voice 108.m4a</t>
+  </si>
+  <si>
+    <t>Voice 109.m4a</t>
+  </si>
+  <si>
+    <t>Voice 110.m4a</t>
+  </si>
+  <si>
+    <t>Voice 111.m4a</t>
+  </si>
+  <si>
+    <t>Voice 112.m4a</t>
+  </si>
+  <si>
+    <t>Voice 113.m4a</t>
+  </si>
+  <si>
+    <t>Voice 114.m4a</t>
+  </si>
+  <si>
+    <t>Voice 115.m4a</t>
+  </si>
+  <si>
+    <t>Voice 116.m4a</t>
+  </si>
+  <si>
+    <t>Voice 117.m4a</t>
+  </si>
+  <si>
+    <t>Voice 118.m4a</t>
+  </si>
+  <si>
+    <t>Voice 119.m4a</t>
+  </si>
+  <si>
+    <t>2018 Jul</t>
+  </si>
+  <si>
+    <t>Voice 120.m4a</t>
+  </si>
+  <si>
+    <t>Voice 121.m4a</t>
+  </si>
+  <si>
+    <t>Voice 122.m4a</t>
+  </si>
+  <si>
+    <t>Voice 123.m4a</t>
+  </si>
+  <si>
+    <t>Voice 124.m4a</t>
+  </si>
+  <si>
+    <t>Voice 125.m4a</t>
+  </si>
+  <si>
+    <t>Voice 126.m4a</t>
+  </si>
+  <si>
+    <t>Voice 127.m4a</t>
+  </si>
+  <si>
+    <t>Voice 128.m4a</t>
+  </si>
+  <si>
+    <t>Voice 129.m4a</t>
+  </si>
+  <si>
+    <t>Voice 130.m4a</t>
+  </si>
+  <si>
+    <t>Voice 131.m4a</t>
+  </si>
+  <si>
+    <t>Voice 132.m4a</t>
+  </si>
+  <si>
+    <t>Voice 133.m4a</t>
+  </si>
+  <si>
+    <t>Voice 134.m4a</t>
+  </si>
+  <si>
+    <t>Voice 135.m4a</t>
+  </si>
+  <si>
+    <t>Voice 136.m4a</t>
+  </si>
+  <si>
+    <t>Voice 137.m4a</t>
+  </si>
+  <si>
+    <t>Voice 138.m4a</t>
+  </si>
+  <si>
+    <t>Voice 139.m4a</t>
+  </si>
+  <si>
+    <t>Voice 140.m4a</t>
+  </si>
+  <si>
+    <t>Voice 141.m4a</t>
+  </si>
+  <si>
+    <t>Voice 142.m4a</t>
+  </si>
+  <si>
+    <t>Voice 143.m4a</t>
+  </si>
+  <si>
+    <t>Voice 144.m4a</t>
+  </si>
+  <si>
+    <t>Voice 145.m4a</t>
+  </si>
+  <si>
+    <t>Voice 146.m4a</t>
+  </si>
+  <si>
+    <t>Voice 147.m4a</t>
+  </si>
+  <si>
+    <t>Voice 148.m4a</t>
+  </si>
+  <si>
+    <t>Voice 149.m4a</t>
+  </si>
+  <si>
+    <t>Voice 150.m4a</t>
+  </si>
+  <si>
+    <t>Voice 151.m4a</t>
+  </si>
+  <si>
+    <t>2018 Aug</t>
+  </si>
+  <si>
+    <t>Voice 152.m4a</t>
+  </si>
+  <si>
+    <t>Voice 153.m4a</t>
+  </si>
+  <si>
+    <t>Voice 154.m4a</t>
+  </si>
+  <si>
+    <t>Voice 155.m4a</t>
+  </si>
+  <si>
+    <t>Voice 159.m4a</t>
+  </si>
+  <si>
+    <t>Voice 162-1h9m23s.m4a</t>
+  </si>
+  <si>
+    <t>2018 Sep</t>
+  </si>
+  <si>
+    <t>Voice 164.m4a</t>
+  </si>
+  <si>
+    <t>Voice 165.m4a</t>
+  </si>
+  <si>
+    <t>Voice 171.m4a</t>
+  </si>
+  <si>
+    <t>Voice 172.m4a</t>
+  </si>
+  <si>
+    <t>Voice 173.m4a</t>
+  </si>
+  <si>
+    <t>Voice 175.m4a</t>
+  </si>
+  <si>
+    <t>Voice 176.m4a</t>
+  </si>
+  <si>
+    <t>Voice 177.m4a</t>
+  </si>
+  <si>
+    <t>Voice 178.m4a</t>
+  </si>
+  <si>
+    <t>Voice 179.m4a</t>
+  </si>
+  <si>
+    <t>2018 Oct</t>
+  </si>
+  <si>
+    <t>Voice 180.m4a</t>
+  </si>
+  <si>
+    <t>Voice 182.m4a</t>
+  </si>
+  <si>
+    <t>Voice 183.m4a</t>
+  </si>
+  <si>
+    <t>Voice 184.m4a</t>
+  </si>
+  <si>
+    <t>Voice 185.m4a</t>
+  </si>
+  <si>
+    <t>Voice 187.m4a</t>
   </si>
 </sst>
 </file>
@@ -2385,7 +2988,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2402,11 +3005,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="9">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
@@ -2443,14 +3056,14 @@
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{27B86026-16DE-4FBC-A7DD-1E3205606A95}" name="Old Name"/>
     <tableColumn id="2" xr3:uid="{984D6489-C759-4F06-8799-56A15D35C943}" name="New Name"/>
-    <tableColumn id="5" xr3:uid="{1AE74ADD-FA71-4CA7-875E-86A15ABC8F0C}" name="_get_name" dataDxfId="5">
+    <tableColumn id="5" xr3:uid="{1AE74ADD-FA71-4CA7-875E-86A15ABC8F0C}" name="_get_name" dataDxfId="8">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Type]]="","Extra",INDEX(_des,MATCH($E2,_num,0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{E86D58B0-08A5-4E08-9156-EF28BD65174B}" name="_name" dataDxfId="4">
+    <tableColumn id="6" xr3:uid="{E86D58B0-08A5-4E08-9156-EF28BD65174B}" name="_name" dataDxfId="7">
       <calculatedColumnFormula>_xlfn.CONCAT(_get_name," ",_find_matches)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{43AEE654-5EDC-4E08-8003-829717A174CE}" name="Type" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{1B832923-B401-4E53-99A6-BDDD132D0DB8}" name="Rename" dataDxfId="2">
+    <tableColumn id="3" xr3:uid="{43AEE654-5EDC-4E08-8003-829717A174CE}" name="Type" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{1B832923-B401-4E53-99A6-BDDD132D0DB8}" name="Rename" dataDxfId="5">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Old Name]]="","",CONCATENATE("ren """,A2,""""," ","""",IF(B2="",D2,B2),IF(Table1[[#This Row],[Type]]="",$J$2,_type),".mp4",""""))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2466,14 +3079,39 @@
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{167D7ECE-9AA6-4D4E-BEE0-95ECC5C73A4E}" name="String"/>
-    <tableColumn id="2" xr3:uid="{EE774F80-BFFB-4579-9A38-529D70AB4F92}" name="Index" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{EE774F80-BFFB-4579-9A38-529D70AB4F92}" name="Index" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{1619E876-8019-475A-8A1F-7973654C9DF1}" name="Name"/>
     <tableColumn id="9" xr3:uid="{942C219C-8025-4154-9A32-587C837A15D8}" name="Author"/>
     <tableColumn id="6" xr3:uid="{805957D0-DCDF-4894-8A65-2A9AEA6C4674}" name="Link"/>
     <tableColumn id="10" xr3:uid="{A69EB3A6-9C46-4964-967F-D28AE4E4FC5D}" name="Lyrics"/>
     <tableColumn id="8" xr3:uid="{FC84D5F9-57C8-4E33-96C4-713B2A3F0DDE}" name="Output"/>
-    <tableColumn id="5" xr3:uid="{78FB681A-89D6-449B-91F7-67AEB87107FA}" name="Audio Output" dataDxfId="0">
+    <tableColumn id="5" xr3:uid="{78FB681A-89D6-449B-91F7-67AEB87107FA}" name="Audio Output" dataDxfId="3">
       <calculatedColumnFormula>_xlfn.CONCAT(B2,"|",E2,"|",C2)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E839C274-D310-4EDB-8585-12B2F4894C90}" name="Table14" displayName="Table14" ref="A1:E17" totalsRowShown="0">
+  <autoFilter ref="A1:E17" xr:uid="{E4C38571-7A30-4A6A-B667-736A6E74B3B0}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E17">
+    <sortCondition ref="D1:D17"/>
+  </sortState>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{A927666E-FC68-42F8-AA1F-8DADEE851989}" name="Data"/>
+    <tableColumn id="2" xr3:uid="{D7F26761-24BE-4166-9343-C05472E8DF12}" name="Old Name" dataDxfId="2">
+      <calculatedColumnFormula>_xlfn.CONCAT(TRIM(MID(SUBSTITUTE(TRIM(Table14[[#This Row],[Data]])," ",REPT(" ",LEN(TRIM(Table14[[#This Row],[Data]])))), (4)*LEN(TRIM(Table14[[#This Row],[Data]]))+1, LEN(TRIM(Table14[[#This Row],[Data]]))))," ",last_word)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{80E73BAC-9F2B-4E9D-AD4D-F268A65A6C4B}" name="Long Date">
+      <calculatedColumnFormula>_xlfn.CONCAT(year," ",month_name," ",day)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{E178FC48-7AD4-4235-A898-931A9747D889}" name="New Name" dataDxfId="1">
+      <calculatedColumnFormula>IF(OR(C2=C1,C2=C3),_xlfn.CONCAT(C2," (",time,").wav"),_xlfn.CONCAT(C2,".wav"))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{36F3EE37-4B49-4C5F-B03B-C3FF7515EB68}" name="Output" dataDxfId="0">
+      <calculatedColumnFormula>SUBSTITUTE(CONCATENATE("ren """,Table14[[#This Row],[Old Name]],""""," ","""",Table14[[#This Row],[New Name]],""""),":","꞉")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -10189,4 +10827,3883 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1741EC65-1BB5-4DA9-8446-6936238EF6AF}">
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>508</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>509</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>510</v>
+      </c>
+      <c r="B2" t="str">
+        <f>_xlfn.CONCAT(TRIM(MID(SUBSTITUTE(TRIM(Table14[[#This Row],[Data]])," ",REPT(" ",LEN(TRIM(Table14[[#This Row],[Data]])))), (4)*LEN(TRIM(Table14[[#This Row],[Data]]))+1, LEN(TRIM(Table14[[#This Row],[Data]]))))," ",last_word)</f>
+        <v>My Recording_1.wav</v>
+      </c>
+      <c r="C2" t="str">
+        <f>_xlfn.CONCAT(year," ",month_name," ",day)</f>
+        <v>2018 Dec 16</v>
+      </c>
+      <c r="D2" s="10" t="str">
+        <f t="shared" ref="D2:D17" si="0">IF(OR(C2=C1,C2=C3),_xlfn.CONCAT(C2," (",time,").wav"),_xlfn.CONCAT(C2,".wav"))</f>
+        <v>2018 Dec 16 (01:34 PM).wav</v>
+      </c>
+      <c r="E2" t="str">
+        <f>SUBSTITUTE(CONCATENATE("ren """,Table14[[#This Row],[Old Name]],""""," ","""",Table14[[#This Row],[New Name]],""""),":","꞉")</f>
+        <v>ren "My Recording_1.wav" "2018 Dec 16 (01꞉34 PM).wav"</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>511</v>
+      </c>
+      <c r="B3" t="s">
+        <v>512</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C2:C17" si="1">_xlfn.CONCAT(year," ",month_name," ",day)</f>
+        <v>2018 Dec 16</v>
+      </c>
+      <c r="D3" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>2018 Dec 16 (10:00 PM).wav</v>
+      </c>
+      <c r="E3" t="str">
+        <f>SUBSTITUTE(CONCATENATE("ren """,Table14[[#This Row],[Old Name]],""""," ","""",Table14[[#This Row],[New Name]],""""),":","꞉")</f>
+        <v>ren "My Recording_3.wav" "2018 Dec 16 (10꞉00 PM).wav"</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>513</v>
+      </c>
+      <c r="B4" t="s">
+        <v>514</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Dec 17</v>
+      </c>
+      <c r="D4" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>2018 Dec 17 (01:54 PM).wav</v>
+      </c>
+      <c r="E4" t="str">
+        <f>SUBSTITUTE(CONCATENATE("ren """,Table14[[#This Row],[Old Name]],""""," ","""",Table14[[#This Row],[New Name]],""""),":","꞉")</f>
+        <v>ren "My Recording_4.wav" "2018 Dec 17 (01꞉54 PM).wav"</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>515</v>
+      </c>
+      <c r="B5" t="s">
+        <v>516</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Dec 17</v>
+      </c>
+      <c r="D5" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>2018 Dec 17 (04:31 PM).wav</v>
+      </c>
+      <c r="E5" t="str">
+        <f>SUBSTITUTE(CONCATENATE("ren """,Table14[[#This Row],[Old Name]],""""," ","""",Table14[[#This Row],[New Name]],""""),":","꞉")</f>
+        <v>ren "My Recording_5.wav" "2018 Dec 17 (04꞉31 PM).wav"</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>517</v>
+      </c>
+      <c r="B6" t="s">
+        <v>518</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Dec 17</v>
+      </c>
+      <c r="D6" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>2018 Dec 17 (11:32 PM).wav</v>
+      </c>
+      <c r="E6" t="str">
+        <f>SUBSTITUTE(CONCATENATE("ren """,Table14[[#This Row],[Old Name]],""""," ","""",Table14[[#This Row],[New Name]],""""),":","꞉")</f>
+        <v>ren "My Recording_6.wav" "2018 Dec 17 (11꞉32 PM).wav"</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>519</v>
+      </c>
+      <c r="B7" t="s">
+        <v>520</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Dec 18</v>
+      </c>
+      <c r="D7" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>2018 Dec 18 (03:47 PM).wav</v>
+      </c>
+      <c r="E7" t="str">
+        <f>SUBSTITUTE(CONCATENATE("ren """,Table14[[#This Row],[Old Name]],""""," ","""",Table14[[#This Row],[New Name]],""""),":","꞉")</f>
+        <v>ren "My Recording_9.wav" "2018 Dec 18 (03꞉47 PM).wav"</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>521</v>
+      </c>
+      <c r="B8" t="s">
+        <v>522</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Dec 18</v>
+      </c>
+      <c r="D8" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>2018 Dec 18 (06:25 PM).wav</v>
+      </c>
+      <c r="E8" t="str">
+        <f>SUBSTITUTE(CONCATENATE("ren """,Table14[[#This Row],[Old Name]],""""," ","""",Table14[[#This Row],[New Name]],""""),":","꞉")</f>
+        <v>ren "My Recording_10.wav" "2018 Dec 18 (06꞉25 PM).wav"</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>523</v>
+      </c>
+      <c r="B9" t="s">
+        <v>524</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Dec 18</v>
+      </c>
+      <c r="D9" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>2018 Dec 18 (07:20 PM).wav</v>
+      </c>
+      <c r="E9" t="str">
+        <f>SUBSTITUTE(CONCATENATE("ren """,Table14[[#This Row],[Old Name]],""""," ","""",Table14[[#This Row],[New Name]],""""),":","꞉")</f>
+        <v>ren "My Recording_11.wav" "2018 Dec 18 (07꞉20 PM).wav"</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>525</v>
+      </c>
+      <c r="B10" t="s">
+        <v>526</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Dec 18</v>
+      </c>
+      <c r="D10" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>2018 Dec 18 (11:21 AM).wav</v>
+      </c>
+      <c r="E10" t="str">
+        <f>SUBSTITUTE(CONCATENATE("ren """,Table14[[#This Row],[Old Name]],""""," ","""",Table14[[#This Row],[New Name]],""""),":","꞉")</f>
+        <v>ren "My Recording_7.wav" "2018 Dec 18 (11꞉21 AM).wav"</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>527</v>
+      </c>
+      <c r="B11" t="s">
+        <v>528</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Dec 18</v>
+      </c>
+      <c r="D11" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>2018 Dec 18 (11:54 AM).wav</v>
+      </c>
+      <c r="E11" t="str">
+        <f>SUBSTITUTE(CONCATENATE("ren """,Table14[[#This Row],[Old Name]],""""," ","""",Table14[[#This Row],[New Name]],""""),":","꞉")</f>
+        <v>ren "My Recording_8.wav" "2018 Dec 18 (11꞉54 AM).wav"</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>529</v>
+      </c>
+      <c r="B12" t="s">
+        <v>530</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Dec 19</v>
+      </c>
+      <c r="D12" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>2018 Dec 19 (01:30 PM).wav</v>
+      </c>
+      <c r="E12" t="str">
+        <f>SUBSTITUTE(CONCATENATE("ren """,Table14[[#This Row],[Old Name]],""""," ","""",Table14[[#This Row],[New Name]],""""),":","꞉")</f>
+        <v>ren "My Recording_15.wav" "2018 Dec 19 (01꞉30 PM).wav"</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>531</v>
+      </c>
+      <c r="B13" t="s">
+        <v>532</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Dec 19</v>
+      </c>
+      <c r="D13" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>2018 Dec 19 (05:18 PM).wav</v>
+      </c>
+      <c r="E13" t="str">
+        <f>SUBSTITUTE(CONCATENATE("ren """,Table14[[#This Row],[Old Name]],""""," ","""",Table14[[#This Row],[New Name]],""""),":","꞉")</f>
+        <v>ren "My Recording_16.wav" "2018 Dec 19 (05꞉18 PM).wav"</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>533</v>
+      </c>
+      <c r="B14" t="s">
+        <v>534</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Dec 19</v>
+      </c>
+      <c r="D14" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>2018 Dec 19 (09:50 PM).wav</v>
+      </c>
+      <c r="E14" t="str">
+        <f>SUBSTITUTE(CONCATENATE("ren """,Table14[[#This Row],[Old Name]],""""," ","""",Table14[[#This Row],[New Name]],""""),":","꞉")</f>
+        <v>ren "My Recording_17.wav" "2018 Dec 19 (09꞉50 PM).wav"</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>535</v>
+      </c>
+      <c r="B15" t="s">
+        <v>536</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Dec 19</v>
+      </c>
+      <c r="D15" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>2018 Dec 19 (10:12 AM).wav</v>
+      </c>
+      <c r="E15" t="str">
+        <f>SUBSTITUTE(CONCATENATE("ren """,Table14[[#This Row],[Old Name]],""""," ","""",Table14[[#This Row],[New Name]],""""),":","꞉")</f>
+        <v>ren "My Recording_13.wav" "2018 Dec 19 (10꞉12 AM).wav"</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>537</v>
+      </c>
+      <c r="B16" t="s">
+        <v>538</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Dec 19</v>
+      </c>
+      <c r="D16" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>2018 Dec 19 (12:30 PM).wav</v>
+      </c>
+      <c r="E16" t="str">
+        <f>SUBSTITUTE(CONCATENATE("ren """,Table14[[#This Row],[Old Name]],""""," ","""",Table14[[#This Row],[New Name]],""""),":","꞉")</f>
+        <v>ren "My Recording_14.wav" "2018 Dec 19 (12꞉30 PM).wav"</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>539</v>
+      </c>
+      <c r="B17" t="s">
+        <v>540</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Dec 19</v>
+      </c>
+      <c r="D17" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>2018 Dec 19 (12:51 AM).wav</v>
+      </c>
+      <c r="E17" t="str">
+        <f>SUBSTITUTE(CONCATENATE("ren """,Table14[[#This Row],[Old Name]],""""," ","""",Table14[[#This Row],[New Name]],""""),":","꞉")</f>
+        <v>ren "My Recording_12.wav" "2018 Dec 19 (12꞉51 AM).wav"</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2D26EA4-95C8-4CE3-9BF1-DCCC41295928}">
+  <dimension ref="A1:K152"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>541</v>
+      </c>
+      <c r="B1" t="s">
+        <v>542</v>
+      </c>
+      <c r="C1">
+        <v>27</v>
+      </c>
+      <c r="D1" t="str">
+        <f>IF(C1="",IF(""="",(-2),(""-1)),"")</f>
+        <v/>
+      </c>
+      <c r="E1" t="str">
+        <f>CONCATENATE(,B1," ",C1,D1)</f>
+        <v>2017 Nov 27</v>
+      </c>
+      <c r="G1" t="str">
+        <f>CONCATENATE("ren """,A1,""""," ","""",E1,$K$1,"""")</f>
+        <v>ren "Voice 021.m4a" "2017 Nov 27.m4a"</v>
+      </c>
+      <c r="K1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>544</v>
+      </c>
+      <c r="B2" t="s">
+        <v>542</v>
+      </c>
+      <c r="C2">
+        <v>27</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ref="D2:D15" si="0">IF(C2=C1,IF(D1="",(-2),(D1-1)),"")</f>
+        <v>-2</v>
+      </c>
+      <c r="E2" t="str">
+        <f t="shared" ref="E2:E65" si="1">CONCATENATE(,B2," ",C2,D2)</f>
+        <v>2017 Nov 27-2</v>
+      </c>
+      <c r="G2" t="str">
+        <f t="shared" ref="G2:G65" si="2">CONCATENATE("ren """,A2,""""," ","""",E2,$K$1,"""")</f>
+        <v>ren "Voice 022.m4a" "2017 Nov 27-2.m4a"</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>545</v>
+      </c>
+      <c r="B3" t="s">
+        <v>542</v>
+      </c>
+      <c r="C3">
+        <v>28</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" si="1"/>
+        <v>2017 Nov 28</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 023.m4a" "2017 Nov 28.m4a"</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>546</v>
+      </c>
+      <c r="B4" t="s">
+        <v>542</v>
+      </c>
+      <c r="C4">
+        <v>29</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="1"/>
+        <v>2017 Nov 29</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 024.m4a" "2017 Nov 29.m4a"</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>547</v>
+      </c>
+      <c r="B5" t="s">
+        <v>542</v>
+      </c>
+      <c r="C5">
+        <v>29</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="1"/>
+        <v>2017 Nov 29-2</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 025.m4a" "2017 Nov 29-2.m4a"</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>548</v>
+      </c>
+      <c r="B6" t="s">
+        <v>542</v>
+      </c>
+      <c r="C6">
+        <v>30</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="1"/>
+        <v>2017 Nov 30</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 026.m4a" "2017 Nov 30.m4a"</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>549</v>
+      </c>
+      <c r="B7" t="s">
+        <v>542</v>
+      </c>
+      <c r="C7">
+        <v>30</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="1"/>
+        <v>2017 Nov 30-2</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 027.m4a" "2017 Nov 30-2.m4a"</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>550</v>
+      </c>
+      <c r="B8" t="s">
+        <v>551</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="1"/>
+        <v>2017 Dec 1</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 028.m4a" "2017 Dec 1.m4a"</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>552</v>
+      </c>
+      <c r="B9" t="s">
+        <v>551</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="1"/>
+        <v>2017 Dec 2</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 029.m4a" "2017 Dec 2.m4a"</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>553</v>
+      </c>
+      <c r="B10" t="s">
+        <v>551</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="1"/>
+        <v>2017 Dec 4</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 030.m4a" "2017 Dec 4.m4a"</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>554</v>
+      </c>
+      <c r="B11" t="s">
+        <v>551</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="1"/>
+        <v>2017 Dec 5</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 031.m4a" "2017 Dec 5.m4a"</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>555</v>
+      </c>
+      <c r="B12" t="s">
+        <v>551</v>
+      </c>
+      <c r="C12">
+        <v>6</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="1"/>
+        <v>2017 Dec 6</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 032.m4a" "2017 Dec 6.m4a"</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>556</v>
+      </c>
+      <c r="B13" t="s">
+        <v>551</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="1"/>
+        <v>2017 Dec 6-2</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 033.m4a" "2017 Dec 6-2.m4a"</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>557</v>
+      </c>
+      <c r="B14" t="s">
+        <v>551</v>
+      </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="1"/>
+        <v>2017 Dec 10</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 034.m4a" "2017 Dec 10.m4a"</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>558</v>
+      </c>
+      <c r="B15" t="s">
+        <v>551</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="1"/>
+        <v>2017 Dec 10-2</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 035.m4a" "2017 Dec 10-2.m4a"</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>559</v>
+      </c>
+      <c r="B16" t="s">
+        <v>551</v>
+      </c>
+      <c r="C16">
+        <v>10</v>
+      </c>
+      <c r="D16">
+        <f>IF(C16=C15,IF(D15="",(-2),(D15-1)),"")</f>
+        <v>-3</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="1"/>
+        <v>2017 Dec 10-3</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 036.m4a" "2017 Dec 10-3.m4a"</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>560</v>
+      </c>
+      <c r="B17" t="s">
+        <v>551</v>
+      </c>
+      <c r="C17">
+        <v>11</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" ref="D17:D80" si="3">IF(C17=C16,IF(D16="",(-2),(D16-1)),"")</f>
+        <v/>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="1"/>
+        <v>2017 Dec 11</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 037.m4a" "2017 Dec 11.m4a"</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>561</v>
+      </c>
+      <c r="B18" t="s">
+        <v>551</v>
+      </c>
+      <c r="C18">
+        <v>12</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="1"/>
+        <v>2017 Dec 12</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 038.m4a" "2017 Dec 12.m4a"</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>562</v>
+      </c>
+      <c r="B19" t="s">
+        <v>551</v>
+      </c>
+      <c r="C19">
+        <v>15</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="1"/>
+        <v>2017 Dec 15</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 039.m4a" "2017 Dec 15.m4a"</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>563</v>
+      </c>
+      <c r="B20" t="s">
+        <v>551</v>
+      </c>
+      <c r="C20">
+        <v>17</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="1"/>
+        <v>2017 Dec 17</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 040.m4a" "2017 Dec 17.m4a"</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>564</v>
+      </c>
+      <c r="B21" t="s">
+        <v>551</v>
+      </c>
+      <c r="C21">
+        <v>17</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="3"/>
+        <v>-2</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="1"/>
+        <v>2017 Dec 17-2</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 041.m4a" "2017 Dec 17-2.m4a"</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>565</v>
+      </c>
+      <c r="B22" t="s">
+        <v>551</v>
+      </c>
+      <c r="C22">
+        <v>17</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="3"/>
+        <v>-3</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="1"/>
+        <v>2017 Dec 17-3</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 042.m4a" "2017 Dec 17-3.m4a"</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>566</v>
+      </c>
+      <c r="B23" t="s">
+        <v>551</v>
+      </c>
+      <c r="C23">
+        <v>17</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="3"/>
+        <v>-4</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="1"/>
+        <v>2017 Dec 17-4</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 043.m4a" "2017 Dec 17-4.m4a"</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>567</v>
+      </c>
+      <c r="B24" t="s">
+        <v>551</v>
+      </c>
+      <c r="C24">
+        <v>24</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="1"/>
+        <v>2017 Dec 24</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 044.m4a" "2017 Dec 24.m4a"</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>568</v>
+      </c>
+      <c r="B25" t="s">
+        <v>551</v>
+      </c>
+      <c r="C25">
+        <v>25</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="1"/>
+        <v>2017 Dec 25</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 045.m4a" "2017 Dec 25.m4a"</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>569</v>
+      </c>
+      <c r="B26" t="s">
+        <v>551</v>
+      </c>
+      <c r="C26">
+        <v>25</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="3"/>
+        <v>-2</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="1"/>
+        <v>2017 Dec 25-2</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 046.m4a" "2017 Dec 25-2.m4a"</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>570</v>
+      </c>
+      <c r="B27" t="s">
+        <v>551</v>
+      </c>
+      <c r="C27">
+        <v>30</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="1"/>
+        <v>2017 Dec 30</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 047.m4a" "2017 Dec 30.m4a"</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>571</v>
+      </c>
+      <c r="B28" t="s">
+        <v>551</v>
+      </c>
+      <c r="C28">
+        <v>30</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="3"/>
+        <v>-2</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="1"/>
+        <v>2017 Dec 30-2</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 048.m4a" "2017 Dec 30-2.m4a"</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>572</v>
+      </c>
+      <c r="B29" t="s">
+        <v>573</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Jan 2</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 049.m4a" "2018 Jan 2.m4a"</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>574</v>
+      </c>
+      <c r="B30" t="s">
+        <v>573</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Jan 3</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 050.m4a" "2018 Jan 3.m4a"</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>575</v>
+      </c>
+      <c r="B31" t="s">
+        <v>573</v>
+      </c>
+      <c r="C31">
+        <v>3</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="3"/>
+        <v>-2</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Jan 3-2</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 051.m4a" "2018 Jan 3-2.m4a"</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>576</v>
+      </c>
+      <c r="B32" t="s">
+        <v>573</v>
+      </c>
+      <c r="C32">
+        <v>5</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Jan 5</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 052.m4a" "2018 Jan 5.m4a"</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>577</v>
+      </c>
+      <c r="B33" t="s">
+        <v>573</v>
+      </c>
+      <c r="C33">
+        <v>5</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="3"/>
+        <v>-2</v>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Jan 5-2</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 053.m4a" "2018 Jan 5-2.m4a"</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>578</v>
+      </c>
+      <c r="B34" t="s">
+        <v>573</v>
+      </c>
+      <c r="C34">
+        <v>7</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E34" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Jan 7</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 054.m4a" "2018 Jan 7.m4a"</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>579</v>
+      </c>
+      <c r="B35" t="s">
+        <v>573</v>
+      </c>
+      <c r="C35">
+        <v>7</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="3"/>
+        <v>-2</v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Jan 7-2</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 055.m4a" "2018 Jan 7-2.m4a"</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>580</v>
+      </c>
+      <c r="B36" t="s">
+        <v>573</v>
+      </c>
+      <c r="C36">
+        <v>7</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="3"/>
+        <v>-3</v>
+      </c>
+      <c r="E36" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Jan 7-3</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 056.m4a" "2018 Jan 7-3.m4a"</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>581</v>
+      </c>
+      <c r="B37" t="s">
+        <v>582</v>
+      </c>
+      <c r="C37">
+        <v>15</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E37" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Feb 15</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 057.m4a" "2018 Feb 15.m4a"</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>583</v>
+      </c>
+      <c r="B38" t="s">
+        <v>582</v>
+      </c>
+      <c r="C38">
+        <v>18</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E38" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Feb 18</v>
+      </c>
+      <c r="G38" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 058.m4a" "2018 Feb 18.m4a"</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>584</v>
+      </c>
+      <c r="B39" t="s">
+        <v>582</v>
+      </c>
+      <c r="C39">
+        <v>21</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E39" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Feb 21</v>
+      </c>
+      <c r="G39" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 059.m4a" "2018 Feb 21.m4a"</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>585</v>
+      </c>
+      <c r="B40" t="s">
+        <v>582</v>
+      </c>
+      <c r="C40">
+        <v>22</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E40" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Feb 22</v>
+      </c>
+      <c r="G40" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 060.m4a" "2018 Feb 22.m4a"</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>586</v>
+      </c>
+      <c r="B41" t="s">
+        <v>582</v>
+      </c>
+      <c r="C41">
+        <v>24</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E41" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Feb 24</v>
+      </c>
+      <c r="G41" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 062.m4a" "2018 Feb 24.m4a"</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>587</v>
+      </c>
+      <c r="B42" t="s">
+        <v>582</v>
+      </c>
+      <c r="C42">
+        <v>24</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="3"/>
+        <v>-2</v>
+      </c>
+      <c r="E42" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Feb 24-2</v>
+      </c>
+      <c r="G42" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 063.m4a" "2018 Feb 24-2.m4a"</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>588</v>
+      </c>
+      <c r="B43" t="s">
+        <v>582</v>
+      </c>
+      <c r="C43">
+        <v>24</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="3"/>
+        <v>-3</v>
+      </c>
+      <c r="E43" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Feb 24-3</v>
+      </c>
+      <c r="G43" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 064.m4a" "2018 Feb 24-3.m4a"</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>589</v>
+      </c>
+      <c r="B44" t="s">
+        <v>582</v>
+      </c>
+      <c r="C44">
+        <v>25</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E44" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Feb 25</v>
+      </c>
+      <c r="G44" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 065.m4a" "2018 Feb 25.m4a"</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>590</v>
+      </c>
+      <c r="B45" t="s">
+        <v>582</v>
+      </c>
+      <c r="C45">
+        <v>25</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="3"/>
+        <v>-2</v>
+      </c>
+      <c r="E45" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Feb 25-2</v>
+      </c>
+      <c r="G45" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 066.m4a" "2018 Feb 25-2.m4a"</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>591</v>
+      </c>
+      <c r="B46" t="s">
+        <v>582</v>
+      </c>
+      <c r="C46">
+        <v>25</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="3"/>
+        <v>-3</v>
+      </c>
+      <c r="E46" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Feb 25-3</v>
+      </c>
+      <c r="G46" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 067.m4a" "2018 Feb 25-3.m4a"</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>592</v>
+      </c>
+      <c r="B47" t="s">
+        <v>593</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E47" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Mar  1</v>
+      </c>
+      <c r="G47" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 068.m4a" "2018 Mar  1.m4a"</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>594</v>
+      </c>
+      <c r="B48" t="s">
+        <v>593</v>
+      </c>
+      <c r="C48">
+        <v>4</v>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E48" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Mar  4</v>
+      </c>
+      <c r="G48" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 069.m4a" "2018 Mar  4.m4a"</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>595</v>
+      </c>
+      <c r="B49" t="s">
+        <v>593</v>
+      </c>
+      <c r="C49">
+        <v>9</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E49" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Mar  9</v>
+      </c>
+      <c r="G49" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 070.m4a" "2018 Mar  9.m4a"</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>596</v>
+      </c>
+      <c r="B50" t="s">
+        <v>593</v>
+      </c>
+      <c r="C50">
+        <v>18</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E50" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Mar  18</v>
+      </c>
+      <c r="G50" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 071.m4a" "2018 Mar  18.m4a"</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>597</v>
+      </c>
+      <c r="B51" t="s">
+        <v>593</v>
+      </c>
+      <c r="C51">
+        <v>20</v>
+      </c>
+      <c r="D51" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E51" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Mar  20</v>
+      </c>
+      <c r="G51" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 072.m4a" "2018 Mar  20.m4a"</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>598</v>
+      </c>
+      <c r="B52" t="s">
+        <v>593</v>
+      </c>
+      <c r="C52">
+        <v>21</v>
+      </c>
+      <c r="D52" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E52" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Mar  21</v>
+      </c>
+      <c r="G52" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 073.m4a" "2018 Mar  21.m4a"</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>599</v>
+      </c>
+      <c r="B53" t="s">
+        <v>593</v>
+      </c>
+      <c r="C53">
+        <v>21</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="3"/>
+        <v>-2</v>
+      </c>
+      <c r="E53" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Mar  21-2</v>
+      </c>
+      <c r="G53" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 074.m4a" "2018 Mar  21-2.m4a"</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>600</v>
+      </c>
+      <c r="B54" t="s">
+        <v>593</v>
+      </c>
+      <c r="C54">
+        <v>22</v>
+      </c>
+      <c r="D54" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E54" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Mar  22</v>
+      </c>
+      <c r="G54" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 075.m4a" "2018 Mar  22.m4a"</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>601</v>
+      </c>
+      <c r="B55" t="s">
+        <v>593</v>
+      </c>
+      <c r="C55">
+        <v>22</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="3"/>
+        <v>-2</v>
+      </c>
+      <c r="E55" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Mar  22-2</v>
+      </c>
+      <c r="G55" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 076.m4a" "2018 Mar  22-2.m4a"</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>602</v>
+      </c>
+      <c r="B56" t="s">
+        <v>593</v>
+      </c>
+      <c r="C56">
+        <v>25</v>
+      </c>
+      <c r="D56" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E56" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Mar  25</v>
+      </c>
+      <c r="G56" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 077.m4a" "2018 Mar  25.m4a"</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>603</v>
+      </c>
+      <c r="B57" t="s">
+        <v>593</v>
+      </c>
+      <c r="C57">
+        <v>26</v>
+      </c>
+      <c r="D57" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E57" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Mar  26</v>
+      </c>
+      <c r="G57" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 078.m4a" "2018 Mar  26.m4a"</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>604</v>
+      </c>
+      <c r="B58" t="s">
+        <v>605</v>
+      </c>
+      <c r="C58">
+        <v>30</v>
+      </c>
+      <c r="D58" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E58" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 Apr 30</v>
+      </c>
+      <c r="G58" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 079.m4a" "2018 Apr 30.m4a"</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>606</v>
+      </c>
+      <c r="B59" t="s">
+        <v>607</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E59" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 May 1</v>
+      </c>
+      <c r="G59" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 080.m4a" "2018 May 1.m4a"</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>608</v>
+      </c>
+      <c r="B60" t="s">
+        <v>607</v>
+      </c>
+      <c r="C60">
+        <v>2</v>
+      </c>
+      <c r="D60" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E60" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 May 2</v>
+      </c>
+      <c r="G60" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 081.m4a" "2018 May 2.m4a"</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>609</v>
+      </c>
+      <c r="B61" t="s">
+        <v>607</v>
+      </c>
+      <c r="C61">
+        <v>3</v>
+      </c>
+      <c r="D61" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E61" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 May 3</v>
+      </c>
+      <c r="G61" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 082.m4a" "2018 May 3.m4a"</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>610</v>
+      </c>
+      <c r="B62" t="s">
+        <v>607</v>
+      </c>
+      <c r="C62">
+        <v>6</v>
+      </c>
+      <c r="D62" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E62" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 May 6</v>
+      </c>
+      <c r="G62" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 083.m4a" "2018 May 6.m4a"</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>611</v>
+      </c>
+      <c r="B63" t="s">
+        <v>607</v>
+      </c>
+      <c r="C63">
+        <v>6</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="3"/>
+        <v>-2</v>
+      </c>
+      <c r="E63" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 May 6-2</v>
+      </c>
+      <c r="G63" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 084.m4a" "2018 May 6-2.m4a"</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>612</v>
+      </c>
+      <c r="B64" t="s">
+        <v>607</v>
+      </c>
+      <c r="C64">
+        <v>6</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="3"/>
+        <v>-3</v>
+      </c>
+      <c r="E64" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 May 6-3</v>
+      </c>
+      <c r="G64" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 085.m4a" "2018 May 6-3.m4a"</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>613</v>
+      </c>
+      <c r="B65" t="s">
+        <v>607</v>
+      </c>
+      <c r="C65">
+        <v>11</v>
+      </c>
+      <c r="D65" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E65" t="str">
+        <f t="shared" si="1"/>
+        <v>2018 May 11</v>
+      </c>
+      <c r="G65" t="str">
+        <f t="shared" si="2"/>
+        <v>ren "Voice 086.m4a" "2018 May 11.m4a"</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>614</v>
+      </c>
+      <c r="B66" t="s">
+        <v>607</v>
+      </c>
+      <c r="C66">
+        <v>11</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="3"/>
+        <v>-2</v>
+      </c>
+      <c r="E66" t="str">
+        <f t="shared" ref="E66:E129" si="4">CONCATENATE(,B66," ",C66,D66)</f>
+        <v>2018 May 11-2</v>
+      </c>
+      <c r="G66" t="str">
+        <f t="shared" ref="G66:G129" si="5">CONCATENATE("ren """,A66,""""," ","""",E66,$K$1,"""")</f>
+        <v>ren "Voice 087.m4a" "2018 May 11-2.m4a"</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>615</v>
+      </c>
+      <c r="B67" t="s">
+        <v>607</v>
+      </c>
+      <c r="C67">
+        <v>22</v>
+      </c>
+      <c r="D67" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E67" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 May 22</v>
+      </c>
+      <c r="G67" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 088.m4a" "2018 May 22.m4a"</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>616</v>
+      </c>
+      <c r="B68" t="s">
+        <v>607</v>
+      </c>
+      <c r="C68">
+        <v>25</v>
+      </c>
+      <c r="D68" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E68" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 May 25</v>
+      </c>
+      <c r="G68" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 089.m4a" "2018 May 25.m4a"</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>617</v>
+      </c>
+      <c r="B69" t="s">
+        <v>607</v>
+      </c>
+      <c r="C69">
+        <v>25</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="3"/>
+        <v>-2</v>
+      </c>
+      <c r="E69" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 May 25-2</v>
+      </c>
+      <c r="G69" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 090.m4a" "2018 May 25-2.m4a"</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>618</v>
+      </c>
+      <c r="B70" t="s">
+        <v>607</v>
+      </c>
+      <c r="C70">
+        <v>27</v>
+      </c>
+      <c r="D70" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E70" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 May 27</v>
+      </c>
+      <c r="G70" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 091.m4a" "2018 May 27.m4a"</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>619</v>
+      </c>
+      <c r="B71" t="s">
+        <v>607</v>
+      </c>
+      <c r="C71">
+        <v>27</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="3"/>
+        <v>-2</v>
+      </c>
+      <c r="E71" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 May 27-2</v>
+      </c>
+      <c r="G71" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 092.m4a" "2018 May 27-2.m4a"</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>620</v>
+      </c>
+      <c r="B72" t="s">
+        <v>607</v>
+      </c>
+      <c r="C72">
+        <v>27</v>
+      </c>
+      <c r="D72">
+        <f t="shared" si="3"/>
+        <v>-3</v>
+      </c>
+      <c r="E72" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 May 27-3</v>
+      </c>
+      <c r="G72" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 093.m4a" "2018 May 27-3.m4a"</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>621</v>
+      </c>
+      <c r="B73" t="s">
+        <v>607</v>
+      </c>
+      <c r="C73">
+        <v>27</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="3"/>
+        <v>-4</v>
+      </c>
+      <c r="E73" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 May 27-4</v>
+      </c>
+      <c r="G73" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 094.m4a" "2018 May 27-4.m4a"</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>622</v>
+      </c>
+      <c r="B74" t="s">
+        <v>607</v>
+      </c>
+      <c r="C74">
+        <v>31</v>
+      </c>
+      <c r="D74" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E74" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 May 31</v>
+      </c>
+      <c r="G74" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 095.m4a" "2018 May 31.m4a"</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>623</v>
+      </c>
+      <c r="B75" t="s">
+        <v>624</v>
+      </c>
+      <c r="C75">
+        <v>1</v>
+      </c>
+      <c r="D75" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E75" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jun 1</v>
+      </c>
+      <c r="G75" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 096.m4a" "2018 Jun 1.m4a"</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>625</v>
+      </c>
+      <c r="B76" t="s">
+        <v>624</v>
+      </c>
+      <c r="C76">
+        <v>3</v>
+      </c>
+      <c r="D76" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E76" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jun 3</v>
+      </c>
+      <c r="G76" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 097.m4a" "2018 Jun 3.m4a"</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>626</v>
+      </c>
+      <c r="B77" t="s">
+        <v>624</v>
+      </c>
+      <c r="C77">
+        <v>3</v>
+      </c>
+      <c r="D77">
+        <f t="shared" si="3"/>
+        <v>-2</v>
+      </c>
+      <c r="E77" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jun 3-2</v>
+      </c>
+      <c r="G77" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 098.m4a" "2018 Jun 3-2.m4a"</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>627</v>
+      </c>
+      <c r="B78" t="s">
+        <v>624</v>
+      </c>
+      <c r="C78">
+        <v>5</v>
+      </c>
+      <c r="D78" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E78" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jun 5</v>
+      </c>
+      <c r="G78" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 099.m4a" "2018 Jun 5.m4a"</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>628</v>
+      </c>
+      <c r="B79" t="s">
+        <v>624</v>
+      </c>
+      <c r="C79">
+        <v>7</v>
+      </c>
+      <c r="D79" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E79" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jun 7</v>
+      </c>
+      <c r="G79" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 100.m4a" "2018 Jun 7.m4a"</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>629</v>
+      </c>
+      <c r="B80" t="s">
+        <v>624</v>
+      </c>
+      <c r="C80">
+        <v>9</v>
+      </c>
+      <c r="D80" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E80" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jun 9</v>
+      </c>
+      <c r="G80" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 101.m4a" "2018 Jun 9.m4a"</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>630</v>
+      </c>
+      <c r="B81" t="s">
+        <v>624</v>
+      </c>
+      <c r="C81">
+        <v>10</v>
+      </c>
+      <c r="D81" t="str">
+        <f t="shared" ref="D81:D144" si="6">IF(C81=C80,IF(D80="",(-2),(D80-1)),"")</f>
+        <v/>
+      </c>
+      <c r="E81" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jun 10</v>
+      </c>
+      <c r="G81" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 102.m4a" "2018 Jun 10.m4a"</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>631</v>
+      </c>
+      <c r="B82" t="s">
+        <v>624</v>
+      </c>
+      <c r="C82">
+        <v>10</v>
+      </c>
+      <c r="D82">
+        <f t="shared" si="6"/>
+        <v>-2</v>
+      </c>
+      <c r="E82" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jun 10-2</v>
+      </c>
+      <c r="G82" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 103.m4a" "2018 Jun 10-2.m4a"</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>632</v>
+      </c>
+      <c r="B83" t="s">
+        <v>624</v>
+      </c>
+      <c r="C83">
+        <v>10</v>
+      </c>
+      <c r="D83">
+        <f t="shared" si="6"/>
+        <v>-3</v>
+      </c>
+      <c r="E83" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jun 10-3</v>
+      </c>
+      <c r="G83" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 104.m4a" "2018 Jun 10-3.m4a"</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>633</v>
+      </c>
+      <c r="B84" t="s">
+        <v>624</v>
+      </c>
+      <c r="C84">
+        <v>10</v>
+      </c>
+      <c r="D84">
+        <f t="shared" si="6"/>
+        <v>-4</v>
+      </c>
+      <c r="E84" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jun 10-4</v>
+      </c>
+      <c r="G84" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 105.m4a" "2018 Jun 10-4.m4a"</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>634</v>
+      </c>
+      <c r="B85" t="s">
+        <v>624</v>
+      </c>
+      <c r="C85">
+        <v>10</v>
+      </c>
+      <c r="D85">
+        <f t="shared" si="6"/>
+        <v>-5</v>
+      </c>
+      <c r="E85" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jun 10-5</v>
+      </c>
+      <c r="G85" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 106.m4a" "2018 Jun 10-5.m4a"</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>635</v>
+      </c>
+      <c r="B86" t="s">
+        <v>624</v>
+      </c>
+      <c r="C86">
+        <v>12</v>
+      </c>
+      <c r="D86" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="E86" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jun 12</v>
+      </c>
+      <c r="G86" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 107.m4a" "2018 Jun 12.m4a"</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>636</v>
+      </c>
+      <c r="B87" t="s">
+        <v>624</v>
+      </c>
+      <c r="C87">
+        <v>12</v>
+      </c>
+      <c r="D87">
+        <f t="shared" si="6"/>
+        <v>-2</v>
+      </c>
+      <c r="E87" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jun 12-2</v>
+      </c>
+      <c r="G87" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 108.m4a" "2018 Jun 12-2.m4a"</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>637</v>
+      </c>
+      <c r="B88" t="s">
+        <v>624</v>
+      </c>
+      <c r="C88">
+        <v>15</v>
+      </c>
+      <c r="D88" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="E88" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jun 15</v>
+      </c>
+      <c r="G88" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 109.m4a" "2018 Jun 15.m4a"</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>638</v>
+      </c>
+      <c r="B89" t="s">
+        <v>624</v>
+      </c>
+      <c r="C89">
+        <v>15</v>
+      </c>
+      <c r="D89">
+        <f t="shared" si="6"/>
+        <v>-2</v>
+      </c>
+      <c r="E89" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jun 15-2</v>
+      </c>
+      <c r="G89" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 110.m4a" "2018 Jun 15-2.m4a"</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>639</v>
+      </c>
+      <c r="B90" t="s">
+        <v>624</v>
+      </c>
+      <c r="C90">
+        <v>16</v>
+      </c>
+      <c r="D90" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="E90" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jun 16</v>
+      </c>
+      <c r="G90" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 111.m4a" "2018 Jun 16.m4a"</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>640</v>
+      </c>
+      <c r="B91" t="s">
+        <v>624</v>
+      </c>
+      <c r="C91">
+        <v>16</v>
+      </c>
+      <c r="D91">
+        <f t="shared" si="6"/>
+        <v>-2</v>
+      </c>
+      <c r="E91" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jun 16-2</v>
+      </c>
+      <c r="G91" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 112.m4a" "2018 Jun 16-2.m4a"</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>641</v>
+      </c>
+      <c r="B92" t="s">
+        <v>624</v>
+      </c>
+      <c r="C92">
+        <v>17</v>
+      </c>
+      <c r="D92" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="E92" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jun 17</v>
+      </c>
+      <c r="G92" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 113.m4a" "2018 Jun 17.m4a"</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>642</v>
+      </c>
+      <c r="B93" t="s">
+        <v>624</v>
+      </c>
+      <c r="C93">
+        <v>17</v>
+      </c>
+      <c r="D93">
+        <f t="shared" si="6"/>
+        <v>-2</v>
+      </c>
+      <c r="E93" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jun 17-2</v>
+      </c>
+      <c r="G93" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 114.m4a" "2018 Jun 17-2.m4a"</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>643</v>
+      </c>
+      <c r="B94" t="s">
+        <v>624</v>
+      </c>
+      <c r="C94">
+        <v>21</v>
+      </c>
+      <c r="D94" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="E94" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jun 21</v>
+      </c>
+      <c r="G94" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 115.m4a" "2018 Jun 21.m4a"</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>644</v>
+      </c>
+      <c r="B95" t="s">
+        <v>624</v>
+      </c>
+      <c r="C95">
+        <v>26</v>
+      </c>
+      <c r="D95" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="E95" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jun 26</v>
+      </c>
+      <c r="G95" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 116.m4a" "2018 Jun 26.m4a"</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>645</v>
+      </c>
+      <c r="B96" t="s">
+        <v>624</v>
+      </c>
+      <c r="C96">
+        <v>26</v>
+      </c>
+      <c r="D96">
+        <f t="shared" si="6"/>
+        <v>-2</v>
+      </c>
+      <c r="E96" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jun 26-2</v>
+      </c>
+      <c r="G96" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 117.m4a" "2018 Jun 26-2.m4a"</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>646</v>
+      </c>
+      <c r="B97" t="s">
+        <v>624</v>
+      </c>
+      <c r="C97">
+        <v>29</v>
+      </c>
+      <c r="D97" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="E97" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jun 29</v>
+      </c>
+      <c r="G97" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 118.m4a" "2018 Jun 29.m4a"</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>647</v>
+      </c>
+      <c r="B98" t="s">
+        <v>648</v>
+      </c>
+      <c r="C98">
+        <v>1</v>
+      </c>
+      <c r="D98" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="E98" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jul 1</v>
+      </c>
+      <c r="G98" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 119.m4a" "2018 Jul 1.m4a"</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>649</v>
+      </c>
+      <c r="B99" t="s">
+        <v>648</v>
+      </c>
+      <c r="C99">
+        <v>1</v>
+      </c>
+      <c r="D99">
+        <f t="shared" si="6"/>
+        <v>-2</v>
+      </c>
+      <c r="E99" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jul 1-2</v>
+      </c>
+      <c r="G99" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 120.m4a" "2018 Jul 1-2.m4a"</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>650</v>
+      </c>
+      <c r="B100" t="s">
+        <v>648</v>
+      </c>
+      <c r="C100">
+        <v>1</v>
+      </c>
+      <c r="D100">
+        <f t="shared" si="6"/>
+        <v>-3</v>
+      </c>
+      <c r="E100" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jul 1-3</v>
+      </c>
+      <c r="G100" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 121.m4a" "2018 Jul 1-3.m4a"</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>651</v>
+      </c>
+      <c r="B101" t="s">
+        <v>648</v>
+      </c>
+      <c r="C101">
+        <v>1</v>
+      </c>
+      <c r="D101">
+        <f t="shared" si="6"/>
+        <v>-4</v>
+      </c>
+      <c r="E101" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jul 1-4</v>
+      </c>
+      <c r="G101" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 122.m4a" "2018 Jul 1-4.m4a"</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>652</v>
+      </c>
+      <c r="B102" t="s">
+        <v>648</v>
+      </c>
+      <c r="C102">
+        <v>6</v>
+      </c>
+      <c r="D102" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="E102" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jul 6</v>
+      </c>
+      <c r="G102" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 123.m4a" "2018 Jul 6.m4a"</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>653</v>
+      </c>
+      <c r="B103" t="s">
+        <v>648</v>
+      </c>
+      <c r="C103">
+        <v>6</v>
+      </c>
+      <c r="D103">
+        <f t="shared" si="6"/>
+        <v>-2</v>
+      </c>
+      <c r="E103" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jul 6-2</v>
+      </c>
+      <c r="G103" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 124.m4a" "2018 Jul 6-2.m4a"</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>654</v>
+      </c>
+      <c r="B104" t="s">
+        <v>648</v>
+      </c>
+      <c r="C104">
+        <v>7</v>
+      </c>
+      <c r="D104" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="E104" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jul 7</v>
+      </c>
+      <c r="G104" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 125.m4a" "2018 Jul 7.m4a"</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>655</v>
+      </c>
+      <c r="B105" t="s">
+        <v>648</v>
+      </c>
+      <c r="C105">
+        <v>7</v>
+      </c>
+      <c r="D105">
+        <f t="shared" si="6"/>
+        <v>-2</v>
+      </c>
+      <c r="E105" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jul 7-2</v>
+      </c>
+      <c r="G105" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 126.m4a" "2018 Jul 7-2.m4a"</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>656</v>
+      </c>
+      <c r="B106" t="s">
+        <v>648</v>
+      </c>
+      <c r="C106">
+        <v>8</v>
+      </c>
+      <c r="D106" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="E106" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jul 8</v>
+      </c>
+      <c r="G106" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 127.m4a" "2018 Jul 8.m4a"</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>657</v>
+      </c>
+      <c r="B107" t="s">
+        <v>648</v>
+      </c>
+      <c r="C107">
+        <v>8</v>
+      </c>
+      <c r="D107">
+        <f t="shared" si="6"/>
+        <v>-2</v>
+      </c>
+      <c r="E107" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jul 8-2</v>
+      </c>
+      <c r="G107" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 128.m4a" "2018 Jul 8-2.m4a"</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>658</v>
+      </c>
+      <c r="B108" t="s">
+        <v>648</v>
+      </c>
+      <c r="C108">
+        <v>10</v>
+      </c>
+      <c r="D108" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="E108" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jul 10</v>
+      </c>
+      <c r="G108" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 129.m4a" "2018 Jul 10.m4a"</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>659</v>
+      </c>
+      <c r="B109" t="s">
+        <v>648</v>
+      </c>
+      <c r="C109">
+        <v>12</v>
+      </c>
+      <c r="D109" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="E109" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jul 12</v>
+      </c>
+      <c r="G109" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 130.m4a" "2018 Jul 12.m4a"</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>660</v>
+      </c>
+      <c r="B110" t="s">
+        <v>648</v>
+      </c>
+      <c r="C110">
+        <v>13</v>
+      </c>
+      <c r="D110" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="E110" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jul 13</v>
+      </c>
+      <c r="G110" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 131.m4a" "2018 Jul 13.m4a"</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>661</v>
+      </c>
+      <c r="B111" t="s">
+        <v>648</v>
+      </c>
+      <c r="C111">
+        <v>14</v>
+      </c>
+      <c r="D111" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="E111" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jul 14</v>
+      </c>
+      <c r="G111" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 132.m4a" "2018 Jul 14.m4a"</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>662</v>
+      </c>
+      <c r="B112" t="s">
+        <v>648</v>
+      </c>
+      <c r="C112">
+        <v>15</v>
+      </c>
+      <c r="D112" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="E112" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jul 15</v>
+      </c>
+      <c r="G112" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 133.m4a" "2018 Jul 15.m4a"</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>663</v>
+      </c>
+      <c r="B113" t="s">
+        <v>648</v>
+      </c>
+      <c r="C113">
+        <v>15</v>
+      </c>
+      <c r="D113">
+        <f t="shared" si="6"/>
+        <v>-2</v>
+      </c>
+      <c r="E113" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jul 15-2</v>
+      </c>
+      <c r="G113" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 134.m4a" "2018 Jul 15-2.m4a"</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>664</v>
+      </c>
+      <c r="B114" t="s">
+        <v>648</v>
+      </c>
+      <c r="C114">
+        <v>15</v>
+      </c>
+      <c r="D114">
+        <f t="shared" si="6"/>
+        <v>-3</v>
+      </c>
+      <c r="E114" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jul 15-3</v>
+      </c>
+      <c r="G114" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 135.m4a" "2018 Jul 15-3.m4a"</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>665</v>
+      </c>
+      <c r="B115" t="s">
+        <v>648</v>
+      </c>
+      <c r="C115">
+        <v>15</v>
+      </c>
+      <c r="D115">
+        <f t="shared" si="6"/>
+        <v>-4</v>
+      </c>
+      <c r="E115" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jul 15-4</v>
+      </c>
+      <c r="G115" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 136.m4a" "2018 Jul 15-4.m4a"</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>666</v>
+      </c>
+      <c r="B116" t="s">
+        <v>648</v>
+      </c>
+      <c r="C116">
+        <v>16</v>
+      </c>
+      <c r="D116" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="E116" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jul 16</v>
+      </c>
+      <c r="G116" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 137.m4a" "2018 Jul 16.m4a"</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>667</v>
+      </c>
+      <c r="B117" t="s">
+        <v>648</v>
+      </c>
+      <c r="C117">
+        <v>17</v>
+      </c>
+      <c r="D117" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="E117" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jul 17</v>
+      </c>
+      <c r="G117" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 138.m4a" "2018 Jul 17.m4a"</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>668</v>
+      </c>
+      <c r="B118" t="s">
+        <v>648</v>
+      </c>
+      <c r="C118">
+        <v>18</v>
+      </c>
+      <c r="D118" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="E118" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jul 18</v>
+      </c>
+      <c r="G118" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 139.m4a" "2018 Jul 18.m4a"</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>669</v>
+      </c>
+      <c r="B119" t="s">
+        <v>648</v>
+      </c>
+      <c r="C119">
+        <v>20</v>
+      </c>
+      <c r="D119" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="E119" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jul 20</v>
+      </c>
+      <c r="G119" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 140.m4a" "2018 Jul 20.m4a"</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>670</v>
+      </c>
+      <c r="B120" t="s">
+        <v>648</v>
+      </c>
+      <c r="C120">
+        <v>21</v>
+      </c>
+      <c r="D120" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="E120" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jul 21</v>
+      </c>
+      <c r="G120" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 141.m4a" "2018 Jul 21.m4a"</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>671</v>
+      </c>
+      <c r="B121" t="s">
+        <v>648</v>
+      </c>
+      <c r="C121">
+        <v>21</v>
+      </c>
+      <c r="D121">
+        <f t="shared" si="6"/>
+        <v>-2</v>
+      </c>
+      <c r="E121" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jul 21-2</v>
+      </c>
+      <c r="G121" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 142.m4a" "2018 Jul 21-2.m4a"</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>672</v>
+      </c>
+      <c r="B122" t="s">
+        <v>648</v>
+      </c>
+      <c r="C122">
+        <v>21</v>
+      </c>
+      <c r="D122">
+        <f t="shared" si="6"/>
+        <v>-3</v>
+      </c>
+      <c r="E122" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jul 21-3</v>
+      </c>
+      <c r="G122" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 143.m4a" "2018 Jul 21-3.m4a"</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>673</v>
+      </c>
+      <c r="B123" t="s">
+        <v>648</v>
+      </c>
+      <c r="C123">
+        <v>22</v>
+      </c>
+      <c r="D123" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="E123" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jul 22</v>
+      </c>
+      <c r="G123" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 144.m4a" "2018 Jul 22.m4a"</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>674</v>
+      </c>
+      <c r="B124" t="s">
+        <v>648</v>
+      </c>
+      <c r="C124">
+        <v>22</v>
+      </c>
+      <c r="D124">
+        <f t="shared" si="6"/>
+        <v>-2</v>
+      </c>
+      <c r="E124" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jul 22-2</v>
+      </c>
+      <c r="G124" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 145.m4a" "2018 Jul 22-2.m4a"</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>675</v>
+      </c>
+      <c r="B125" t="s">
+        <v>648</v>
+      </c>
+      <c r="C125">
+        <v>22</v>
+      </c>
+      <c r="D125">
+        <f t="shared" si="6"/>
+        <v>-3</v>
+      </c>
+      <c r="E125" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jul 22-3</v>
+      </c>
+      <c r="G125" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 146.m4a" "2018 Jul 22-3.m4a"</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>676</v>
+      </c>
+      <c r="B126" t="s">
+        <v>648</v>
+      </c>
+      <c r="C126">
+        <v>22</v>
+      </c>
+      <c r="D126">
+        <f t="shared" si="6"/>
+        <v>-4</v>
+      </c>
+      <c r="E126" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jul 22-4</v>
+      </c>
+      <c r="G126" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 147.m4a" "2018 Jul 22-4.m4a"</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>677</v>
+      </c>
+      <c r="B127" t="s">
+        <v>648</v>
+      </c>
+      <c r="C127">
+        <v>22</v>
+      </c>
+      <c r="D127">
+        <f t="shared" si="6"/>
+        <v>-5</v>
+      </c>
+      <c r="E127" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jul 22-5</v>
+      </c>
+      <c r="G127" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 148.m4a" "2018 Jul 22-5.m4a"</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>678</v>
+      </c>
+      <c r="B128" t="s">
+        <v>648</v>
+      </c>
+      <c r="C128">
+        <v>22</v>
+      </c>
+      <c r="D128">
+        <f t="shared" si="6"/>
+        <v>-6</v>
+      </c>
+      <c r="E128" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jul 22-6</v>
+      </c>
+      <c r="G128" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 149.m4a" "2018 Jul 22-6.m4a"</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>679</v>
+      </c>
+      <c r="B129" t="s">
+        <v>648</v>
+      </c>
+      <c r="C129">
+        <v>28</v>
+      </c>
+      <c r="D129" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="E129" t="str">
+        <f t="shared" si="4"/>
+        <v>2018 Jul 28</v>
+      </c>
+      <c r="G129" t="str">
+        <f t="shared" si="5"/>
+        <v>ren "Voice 150.m4a" "2018 Jul 28.m4a"</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>680</v>
+      </c>
+      <c r="B130" t="s">
+        <v>681</v>
+      </c>
+      <c r="C130">
+        <v>2</v>
+      </c>
+      <c r="D130" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="E130" t="str">
+        <f t="shared" ref="E130:E152" si="7">CONCATENATE(,B130," ",C130,D130)</f>
+        <v>2018 Aug 2</v>
+      </c>
+      <c r="G130" t="str">
+        <f t="shared" ref="G130:G152" si="8">CONCATENATE("ren """,A130,""""," ","""",E130,$K$1,"""")</f>
+        <v>ren "Voice 151.m4a" "2018 Aug 2.m4a"</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>682</v>
+      </c>
+      <c r="B131" t="s">
+        <v>681</v>
+      </c>
+      <c r="C131">
+        <v>4</v>
+      </c>
+      <c r="D131" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="E131" t="str">
+        <f t="shared" si="7"/>
+        <v>2018 Aug 4</v>
+      </c>
+      <c r="G131" t="str">
+        <f t="shared" si="8"/>
+        <v>ren "Voice 152.m4a" "2018 Aug 4.m4a"</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>683</v>
+      </c>
+      <c r="B132" t="s">
+        <v>681</v>
+      </c>
+      <c r="C132">
+        <v>5</v>
+      </c>
+      <c r="D132" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="E132" t="str">
+        <f t="shared" si="7"/>
+        <v>2018 Aug 5</v>
+      </c>
+      <c r="G132" t="str">
+        <f t="shared" si="8"/>
+        <v>ren "Voice 153.m4a" "2018 Aug 5.m4a"</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>684</v>
+      </c>
+      <c r="B133" t="s">
+        <v>681</v>
+      </c>
+      <c r="C133">
+        <v>5</v>
+      </c>
+      <c r="D133">
+        <f t="shared" si="6"/>
+        <v>-2</v>
+      </c>
+      <c r="E133" t="str">
+        <f t="shared" si="7"/>
+        <v>2018 Aug 5-2</v>
+      </c>
+      <c r="G133" t="str">
+        <f t="shared" si="8"/>
+        <v>ren "Voice 154.m4a" "2018 Aug 5-2.m4a"</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>685</v>
+      </c>
+      <c r="B134" t="s">
+        <v>681</v>
+      </c>
+      <c r="C134">
+        <v>5</v>
+      </c>
+      <c r="D134">
+        <f t="shared" si="6"/>
+        <v>-3</v>
+      </c>
+      <c r="E134" t="str">
+        <f t="shared" si="7"/>
+        <v>2018 Aug 5-3</v>
+      </c>
+      <c r="G134" t="str">
+        <f t="shared" si="8"/>
+        <v>ren "Voice 155.m4a" "2018 Aug 5-3.m4a"</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>686</v>
+      </c>
+      <c r="B135" t="s">
+        <v>681</v>
+      </c>
+      <c r="C135">
+        <v>12</v>
+      </c>
+      <c r="D135" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="E135" t="str">
+        <f t="shared" si="7"/>
+        <v>2018 Aug 12</v>
+      </c>
+      <c r="G135" t="str">
+        <f t="shared" si="8"/>
+        <v>ren "Voice 159.m4a" "2018 Aug 12.m4a"</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>687</v>
+      </c>
+      <c r="B136" t="s">
+        <v>688</v>
+      </c>
+      <c r="C136">
+        <v>1</v>
+      </c>
+      <c r="D136" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="E136" t="str">
+        <f t="shared" si="7"/>
+        <v>2018 Sep 1</v>
+      </c>
+      <c r="G136" t="str">
+        <f>CONCATENATE("ren """,A136,""""," ","""",E136,"-1h9m23s.m4a","""")</f>
+        <v>ren "Voice 162-1h9m23s.m4a" "2018 Sep 1-1h9m23s.m4a"</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>689</v>
+      </c>
+      <c r="B137" t="s">
+        <v>688</v>
+      </c>
+      <c r="C137">
+        <v>1</v>
+      </c>
+      <c r="D137">
+        <f t="shared" si="6"/>
+        <v>-2</v>
+      </c>
+      <c r="E137" t="str">
+        <f t="shared" si="7"/>
+        <v>2018 Sep 1-2</v>
+      </c>
+      <c r="G137" t="str">
+        <f t="shared" si="8"/>
+        <v>ren "Voice 164.m4a" "2018 Sep 1-2.m4a"</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>690</v>
+      </c>
+      <c r="B138" t="s">
+        <v>688</v>
+      </c>
+      <c r="C138">
+        <v>2</v>
+      </c>
+      <c r="D138" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="E138" t="str">
+        <f t="shared" si="7"/>
+        <v>2018 Sep 2</v>
+      </c>
+      <c r="G138" t="str">
+        <f t="shared" si="8"/>
+        <v>ren "Voice 165.m4a" "2018 Sep 2.m4a"</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>691</v>
+      </c>
+      <c r="B139" t="s">
+        <v>688</v>
+      </c>
+      <c r="C139">
+        <v>19</v>
+      </c>
+      <c r="D139" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="E139" t="str">
+        <f t="shared" si="7"/>
+        <v>2018 Sep 19</v>
+      </c>
+      <c r="G139" t="str">
+        <f t="shared" si="8"/>
+        <v>ren "Voice 171.m4a" "2018 Sep 19.m4a"</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>692</v>
+      </c>
+      <c r="B140" t="s">
+        <v>688</v>
+      </c>
+      <c r="C140">
+        <v>20</v>
+      </c>
+      <c r="D140" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="E140" t="str">
+        <f t="shared" si="7"/>
+        <v>2018 Sep 20</v>
+      </c>
+      <c r="G140" t="str">
+        <f t="shared" si="8"/>
+        <v>ren "Voice 172.m4a" "2018 Sep 20.m4a"</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>693</v>
+      </c>
+      <c r="B141" t="s">
+        <v>688</v>
+      </c>
+      <c r="C141">
+        <v>21</v>
+      </c>
+      <c r="D141" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="E141" t="str">
+        <f t="shared" si="7"/>
+        <v>2018 Sep 21</v>
+      </c>
+      <c r="G141" t="str">
+        <f t="shared" si="8"/>
+        <v>ren "Voice 173.m4a" "2018 Sep 21.m4a"</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>694</v>
+      </c>
+      <c r="B142" t="s">
+        <v>688</v>
+      </c>
+      <c r="C142">
+        <v>26</v>
+      </c>
+      <c r="D142" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="E142" t="str">
+        <f t="shared" si="7"/>
+        <v>2018 Sep 26</v>
+      </c>
+      <c r="G142" t="str">
+        <f t="shared" si="8"/>
+        <v>ren "Voice 175.m4a" "2018 Sep 26.m4a"</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>695</v>
+      </c>
+      <c r="B143" t="s">
+        <v>688</v>
+      </c>
+      <c r="C143">
+        <v>26</v>
+      </c>
+      <c r="D143">
+        <f t="shared" si="6"/>
+        <v>-2</v>
+      </c>
+      <c r="E143" t="str">
+        <f t="shared" si="7"/>
+        <v>2018 Sep 26-2</v>
+      </c>
+      <c r="G143" t="str">
+        <f t="shared" si="8"/>
+        <v>ren "Voice 176.m4a" "2018 Sep 26-2.m4a"</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>696</v>
+      </c>
+      <c r="B144" t="s">
+        <v>688</v>
+      </c>
+      <c r="C144">
+        <v>29</v>
+      </c>
+      <c r="D144" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="E144" t="str">
+        <f t="shared" si="7"/>
+        <v>2018 Sep 29</v>
+      </c>
+      <c r="G144" t="str">
+        <f t="shared" si="8"/>
+        <v>ren "Voice 177.m4a" "2018 Sep 29.m4a"</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>697</v>
+      </c>
+      <c r="B145" t="s">
+        <v>688</v>
+      </c>
+      <c r="C145">
+        <v>30</v>
+      </c>
+      <c r="D145" t="str">
+        <f t="shared" ref="D145:D152" si="9">IF(C145=C144,IF(D144="",(-2),(D144-1)),"")</f>
+        <v/>
+      </c>
+      <c r="E145" t="str">
+        <f t="shared" si="7"/>
+        <v>2018 Sep 30</v>
+      </c>
+      <c r="G145" t="str">
+        <f t="shared" si="8"/>
+        <v>ren "Voice 178.m4a" "2018 Sep 30.m4a"</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>698</v>
+      </c>
+      <c r="B146" t="s">
+        <v>699</v>
+      </c>
+      <c r="C146">
+        <v>1</v>
+      </c>
+      <c r="D146" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="E146" t="str">
+        <f t="shared" si="7"/>
+        <v>2018 Oct 1</v>
+      </c>
+      <c r="G146" t="str">
+        <f t="shared" si="8"/>
+        <v>ren "Voice 179.m4a" "2018 Oct 1.m4a"</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>700</v>
+      </c>
+      <c r="B147" t="s">
+        <v>699</v>
+      </c>
+      <c r="C147">
+        <v>6</v>
+      </c>
+      <c r="D147" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="E147" t="str">
+        <f t="shared" si="7"/>
+        <v>2018 Oct 6</v>
+      </c>
+      <c r="G147" t="str">
+        <f t="shared" si="8"/>
+        <v>ren "Voice 180.m4a" "2018 Oct 6.m4a"</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>701</v>
+      </c>
+      <c r="B148" t="s">
+        <v>699</v>
+      </c>
+      <c r="C148">
+        <v>7</v>
+      </c>
+      <c r="D148" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="E148" t="str">
+        <f t="shared" si="7"/>
+        <v>2018 Oct 7</v>
+      </c>
+      <c r="G148" t="str">
+        <f t="shared" si="8"/>
+        <v>ren "Voice 182.m4a" "2018 Oct 7.m4a"</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>702</v>
+      </c>
+      <c r="B149" t="s">
+        <v>699</v>
+      </c>
+      <c r="C149">
+        <v>12</v>
+      </c>
+      <c r="D149" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="E149" t="str">
+        <f t="shared" si="7"/>
+        <v>2018 Oct 12</v>
+      </c>
+      <c r="G149" t="str">
+        <f t="shared" si="8"/>
+        <v>ren "Voice 183.m4a" "2018 Oct 12.m4a"</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>703</v>
+      </c>
+      <c r="B150" t="s">
+        <v>699</v>
+      </c>
+      <c r="C150">
+        <v>13</v>
+      </c>
+      <c r="D150" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="E150" t="str">
+        <f t="shared" si="7"/>
+        <v>2018 Oct 13</v>
+      </c>
+      <c r="G150" t="str">
+        <f t="shared" si="8"/>
+        <v>ren "Voice 184.m4a" "2018 Oct 13.m4a"</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>704</v>
+      </c>
+      <c r="B151" t="s">
+        <v>699</v>
+      </c>
+      <c r="C151">
+        <v>13</v>
+      </c>
+      <c r="D151">
+        <f t="shared" si="9"/>
+        <v>-2</v>
+      </c>
+      <c r="E151" t="str">
+        <f t="shared" si="7"/>
+        <v>2018 Oct 13-2</v>
+      </c>
+      <c r="G151" t="str">
+        <f t="shared" si="8"/>
+        <v>ren "Voice 185.m4a" "2018 Oct 13-2.m4a"</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>705</v>
+      </c>
+      <c r="B152" t="s">
+        <v>699</v>
+      </c>
+      <c r="C152">
+        <v>13</v>
+      </c>
+      <c r="D152">
+        <f t="shared" si="9"/>
+        <v>-3</v>
+      </c>
+      <c r="E152" t="str">
+        <f t="shared" si="7"/>
+        <v>2018 Oct 13-3</v>
+      </c>
+      <c r="G152" t="str">
+        <f t="shared" si="8"/>
+        <v>ren "Voice 187.m4a" "2018 Oct 13-3.m4a"</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>